<commit_message>
Update API_test expected results, after merging develop
</commit_message>
<xml_diff>
--- a/landbosse/landbosse_api/API_test/project_list.xlsx
+++ b/landbosse/landbosse_api/API_test/project_list.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/landbosse/landbosse_api/API_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8E710D-1ED0-AC46-9FB7-FF6105E015D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FE962B-454F-C74E-9595-8099C0C3FCD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1280" windowWidth="28800" windowHeight="10960" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14360" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Project list" sheetId="1" r:id="rId1"/>
-    <sheet name="Parametric list" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Project ID</t>
   </si>
@@ -79,12 +86,12 @@
     <t>Combined Homerun Trench Length to Substation (km)</t>
   </si>
   <si>
+    <t>50-year Gust Velocity (m/s)</t>
+  </si>
+  <si>
     <t>Total project construction time (months)</t>
   </si>
   <si>
-    <t>50-year Gust Velocity (m/s)</t>
-  </si>
-  <si>
     <t>Non-Erection Wind Delay Critical Height (m)</t>
   </si>
   <si>
@@ -109,52 +116,61 @@
     <t>Percent of roads that will be constructed</t>
   </si>
   <si>
+    <t>Road width (ft)</t>
+  </si>
+  <si>
+    <t>Road thickness (in)</t>
+  </si>
+  <si>
+    <t>Crane width (m)</t>
+  </si>
+  <si>
+    <t>Number of highway permits</t>
+  </si>
+  <si>
+    <t>Number of access roads</t>
+  </si>
+  <si>
+    <t>Overtime multiplier</t>
+  </si>
+  <si>
+    <t>Allow same flag</t>
+  </si>
+  <si>
+    <t>Markup contingency</t>
+  </si>
+  <si>
+    <t>Markup warranty management</t>
+  </si>
+  <si>
+    <t>Markup sales and use tax</t>
+  </si>
+  <si>
+    <t>Markup overhead</t>
+  </si>
+  <si>
+    <t>Markup profit margin</t>
+  </si>
+  <si>
+    <t>Project data file</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Calculate road cost for distributed wind? (y/n)</t>
+  </si>
+  <si>
     <t>y</t>
   </si>
   <si>
-    <t>project_1</t>
-  </si>
-  <si>
-    <t>Road width (ft)</t>
-  </si>
-  <si>
-    <t>Road thickness (in)</t>
-  </si>
-  <si>
-    <t>Crane width (m)</t>
-  </si>
-  <si>
-    <t>Number of highway permits</t>
-  </si>
-  <si>
-    <t>Number of access roads</t>
-  </si>
-  <si>
-    <t>Overtime multiplier</t>
-  </si>
-  <si>
-    <t>Allow same flag</t>
-  </si>
-  <si>
-    <t>Markup contingency</t>
-  </si>
-  <si>
-    <t>Markup warranty management</t>
-  </si>
-  <si>
-    <t>Markup sales and use tax</t>
-  </si>
-  <si>
-    <t>Markup overhead</t>
-  </si>
-  <si>
-    <t>Markup profit margin</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Project data file</t>
+    <t>Site prep area for Distributed wind (m2)</t>
+  </si>
+  <si>
+    <t>Override total management cost for distributed (0 does not override)</t>
+  </si>
+  <si>
+    <t>Utility Interconnection Fees (Small DW only)</t>
   </si>
   <si>
     <t>Labor cost multiplier</t>
@@ -163,14 +179,20 @@
     <t>Crane breakdown fraction</t>
   </si>
   <si>
-    <t>project_data_defaults_test</t>
+    <t>ge15_public</t>
+  </si>
+  <si>
+    <t>foundation_validation_ge15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -181,6 +203,19 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,19 +238,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -527,54 +568,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AT5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="28.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="53.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="46.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18" style="1" customWidth="1"/>
+    <col min="18" max="18" width="27.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="52.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="46" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.5" style="1" customWidth="1"/>
+    <col min="22" max="22" width="39.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="1"/>
+    <col min="26" max="26" width="20" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.1640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="25.5" style="1" customWidth="1"/>
+    <col min="31" max="31" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="39.6640625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="23" style="1" customWidth="1"/>
+    <col min="34" max="34" width="27.5" style="1" customWidth="1"/>
+    <col min="35" max="35" width="22.1640625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="24.6640625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="26.6640625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="60.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="32" style="1" customWidth="1"/>
+    <col min="40" max="40" width="27.1640625" style="1" customWidth="1"/>
+    <col min="41" max="41" width="22.6640625" style="1" customWidth="1"/>
+    <col min="42" max="42" width="34" style="1" customWidth="1"/>
+    <col min="43" max="43" width="24.6640625" style="1" customWidth="1"/>
+    <col min="44" max="44" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -616,7 +674,7 @@
         <v>12</v>
       </c>
       <c r="Q1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R1" t="s">
         <v>13</v>
@@ -633,210 +691,231 @@
       <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AH1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AI1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AK1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AL1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AN1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AO1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AP1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>44</v>
+      <c r="AR1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1">
         <v>9</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="1">
         <v>1.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>80</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>77</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>10</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>100</v>
       </c>
-      <c r="J2">
-        <v>0.7</v>
-      </c>
-      <c r="K2">
+      <c r="J2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="1">
         <v>1.5</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>0.2</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>2.36</v>
       </c>
       <c r="O2" s="3">
         <v>589000</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="1">
         <v>191521</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="1">
         <v>59.5</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="1">
         <v>60</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="1">
         <v>0</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="1">
         <v>50</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="1">
         <v>10</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="1">
         <v>15</v>
       </c>
-      <c r="W2">
-        <v>10</v>
-      </c>
-      <c r="X2">
-        <v>137</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z2">
+      <c r="W2" s="2">
+        <v>5</v>
+      </c>
+      <c r="X2" s="2">
+        <v>130</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" s="2">
         <v>5000</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="2">
         <v>0.6</v>
       </c>
       <c r="AB2" s="4">
         <v>0.33</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="2">
         <v>20</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="2">
         <v>8</v>
       </c>
-      <c r="AE2">
-        <v>11</v>
-      </c>
-      <c r="AF2">
+      <c r="AE2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="AH2" s="2">
         <v>10</v>
       </c>
-      <c r="AG2">
+      <c r="AI2" s="2">
         <v>2</v>
       </c>
-      <c r="AH2">
+      <c r="AJ2" s="2">
         <v>1.4</v>
       </c>
-      <c r="AI2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ2">
+      <c r="AK2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="2">
         <v>0.03</v>
       </c>
-      <c r="AK2">
+      <c r="AN2" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="AL2">
+      <c r="AO2" s="2">
         <v>0</v>
       </c>
-      <c r="AM2">
+      <c r="AP2" s="2">
         <v>0.05</v>
       </c>
-      <c r="AN2">
+      <c r="AQ2" s="2">
         <v>0.05</v>
       </c>
-      <c r="AO2">
+      <c r="AR2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="2">
         <v>1</v>
       </c>
-      <c r="AP2">
+      <c r="AT2" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A3"/>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="Z5" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="HadWk4PfJwN1iONNxk8yt4zaSrngLJdhi/S+d6msPftxWtYUbIwtIqYMPOe1v+0fQdA59yA84CT8ADfRpTtRTA==" saltValue="JZptj2PlSb2KhidwOtH/SQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E92228-1010-354F-B5D5-9F3A45BA98AD}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>